<commit_message>
ajout card totaux stat + membres + divers fix
</commit_message>
<xml_diff>
--- a/www/asso_donation_forest.xlsx
+++ b/www/asso_donation_forest.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
   <si>
     <t>Id</t>
   </si>
@@ -35,45 +35,6 @@
     <t>Date enregistrement</t>
   </si>
   <si>
-    <t>Linda</t>
-  </si>
-  <si>
-    <t>2019-04-24 16:06:43</t>
-  </si>
-  <si>
-    <t>2019-04-24 16:06:40</t>
-  </si>
-  <si>
-    <t>2019-04-24 16:06:38</t>
-  </si>
-  <si>
-    <t>2019-04-24 16:06:34</t>
-  </si>
-  <si>
-    <t>2019-04-24 16:06:31</t>
-  </si>
-  <si>
-    <t>2019-04-24 14:47:32</t>
-  </si>
-  <si>
-    <t>2019-04-24 14:47:30</t>
-  </si>
-  <si>
-    <t>2019-04-24 14:47:27</t>
-  </si>
-  <si>
-    <t>2019-04-24 14:47:24</t>
-  </si>
-  <si>
-    <t>2019-04-24 14:47:21</t>
-  </si>
-  <si>
-    <t>2019-04-24 14:47:18</t>
-  </si>
-  <si>
-    <t>2019-04-24 14:47:15</t>
-  </si>
-  <si>
     <t>Joelle</t>
   </si>
   <si>
@@ -84,9 +45,6 @@
   </si>
   <si>
     <t>2019-04-19 06:43:30</t>
-  </si>
-  <si>
-    <t>2019-04-18 14:48:16</t>
   </si>
   <si>
     <t>2019-01-01 00:01:00</t>
@@ -428,7 +386,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +394,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,288 +414,64 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:6">
       <c r="A2">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B2">
-        <v>6311</v>
+        <v>1340</v>
       </c>
       <c r="C2" t="s">
         <v>6</v>
       </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
       <c r="E2">
-        <v>2414</v>
+        <v>123</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:6">
       <c r="A3">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B3">
-        <v>6311</v>
+        <v>1340</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
       <c r="E3">
-        <v>12424</v>
+        <v>333</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:6">
       <c r="A4">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="B4">
-        <v>6311</v>
+        <v>1340</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
       <c r="E4">
-        <v>423432</v>
+        <v>1111</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5">
-        <v>115</v>
-      </c>
-      <c r="B5">
-        <v>6311</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5">
-        <v>1244</v>
-      </c>
-      <c r="F5" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6">
-        <v>114</v>
-      </c>
-      <c r="B6">
-        <v>6311</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E6">
-        <v>123</v>
-      </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7">
-        <v>113</v>
-      </c>
-      <c r="B7">
-        <v>6311</v>
-      </c>
-      <c r="C7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7">
-        <v>8888</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8">
-        <v>112</v>
-      </c>
-      <c r="B8">
-        <v>6311</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>1111</v>
-      </c>
-      <c r="F8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9">
-        <v>111</v>
-      </c>
-      <c r="B9">
-        <v>6311</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9">
-        <v>2222</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10">
-        <v>110</v>
-      </c>
-      <c r="B10">
-        <v>6311</v>
-      </c>
-      <c r="C10" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10">
-        <v>3333</v>
-      </c>
-      <c r="F10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11">
-        <v>109</v>
-      </c>
-      <c r="B11">
-        <v>6311</v>
-      </c>
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11">
-        <v>6666</v>
-      </c>
-      <c r="F11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12">
-        <v>108</v>
-      </c>
-      <c r="B12">
-        <v>6311</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12">
-        <v>666</v>
-      </c>
-      <c r="F12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13">
-        <v>107</v>
-      </c>
-      <c r="B13">
-        <v>6311</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
-      </c>
-      <c r="E13">
-        <v>777</v>
-      </c>
-      <c r="F13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14">
-        <v>106</v>
-      </c>
-      <c r="B14">
-        <v>1340</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14">
-        <v>123</v>
-      </c>
-      <c r="F14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15">
-        <v>103</v>
-      </c>
-      <c r="B15">
-        <v>1340</v>
-      </c>
-      <c r="C15" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15">
-        <v>333</v>
-      </c>
-      <c r="F15" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16">
-        <v>100</v>
-      </c>
-      <c r="B16">
-        <v>6311</v>
-      </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16">
-        <v>111111</v>
-      </c>
-      <c r="F16" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17">
-        <v>99</v>
-      </c>
-      <c r="B17">
-        <v>1340</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17">
-        <v>1111</v>
-      </c>
-      <c r="F17" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>